<commit_message>
update commit non ideal_gas.java
</commit_message>
<xml_diff>
--- a/oop_chart.xlsx
+++ b/oop_chart.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\MiniProject_Java\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\Programming Language Study\java_miniproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7D85CE-8EA6-424E-A865-3205331354DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BA4056-EF30-44C6-AD90-451F9B169E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5E904299-E32A-4B5E-ABBF-A927AB0918F1}"/>
   </bookViews>
@@ -36,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>mol_calculate</t>
   </si>
   <si>
     <t>inten_solu_calculate</t>
-  </si>
-  <si>
-    <t>pressure()
-volume()
-mol()
-tempereture()</t>
   </si>
   <si>
     <t>mol_calculate()
@@ -74,9 +68,6 @@
   </si>
   <si>
     <t>molal_calc</t>
-  </si>
-  <si>
-    <t>ideal_gas_cal</t>
   </si>
   <si>
     <t xml:space="preserve"> +mass()
@@ -252,9 +243,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -270,12 +258,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -287,6 +269,15 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -411,56 +402,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>191900</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>161048</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>199431</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>161048</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="Straight Connector 9">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD0B59DF-7C1C-4715-B325-9FD2CBAB7D1A}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="17200829" y="6362017"/>
-          <a:ext cx="7531" cy="845587"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>670643</xdr:colOff>
       <xdr:row>36</xdr:row>
@@ -487,56 +428,6 @@
         <a:xfrm>
           <a:off x="5785568" y="12848348"/>
           <a:ext cx="7406557" cy="0"/>
-        </a:xfrm>
-        <a:prstGeom prst="line">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>411970</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>74042</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>413461</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>86161</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="21" name="Straight Connector 20">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0050DE0F-CD3D-4C6A-B885-6BC40A83578C}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvCxnSpPr/>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipH="1">
-          <a:off x="21763845" y="11599292"/>
-          <a:ext cx="1491" cy="1059869"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -1757,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60F5A653-5B1D-4963-95C9-716C7C4CE490}">
   <dimension ref="D12:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M34" sqref="M34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="25.5703125" defaultRowHeight="27.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1776,165 +1667,160 @@
   <sheetData>
     <row r="12" spans="6:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F12" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="6:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F13" s="9" t="s">
-        <v>16</v>
+      <c r="F13" s="8" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="6:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F14" s="10"/>
+      <c r="F14" s="9"/>
       <c r="J14" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="6:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F15" s="11"/>
-      <c r="J15" s="9" t="s">
-        <v>21</v>
+      <c r="F15" s="10"/>
+      <c r="J15" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="6:10" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="17"/>
+      <c r="J16" s="14"/>
     </row>
     <row r="17" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J17" s="7" t="s">
-        <v>22</v>
+        <v>5</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="F18" s="9" t="s">
-        <v>17</v>
+      <c r="F18" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="J18" s="7"/>
     </row>
     <row r="19" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="F19" s="16"/>
-      <c r="H19" s="9" t="s">
-        <v>20</v>
+      <c r="D19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="13"/>
+      <c r="H19" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D20" s="8"/>
-      <c r="F20" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="10"/>
+      <c r="D20" s="7"/>
+      <c r="F20" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="9"/>
     </row>
     <row r="21" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D21" s="8"/>
-      <c r="F21" s="16"/>
-      <c r="H21" s="10"/>
+      <c r="D21" s="7"/>
+      <c r="F21" s="13"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D22" s="8"/>
+      <c r="D22" s="7"/>
       <c r="F22" s="2"/>
-      <c r="H22" s="10"/>
+      <c r="H22" s="9"/>
       <c r="J22" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="23" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="8"/>
+      <c r="D23" s="7"/>
       <c r="F23" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="J23" s="9" t="s">
-        <v>23</v>
+        <v>6</v>
+      </c>
+      <c r="H23" s="10"/>
+      <c r="J23" s="8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F24" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="J24" s="17"/>
+      <c r="F24" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J24" s="14"/>
     </row>
     <row r="25" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F25" s="8"/>
-      <c r="J25" s="7" t="s">
-        <v>24</v>
+      <c r="F25" s="7"/>
+      <c r="J25" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="26" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F26" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J26" s="8"/>
+        <v>12</v>
+      </c>
+      <c r="J26" s="7"/>
     </row>
     <row r="27" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M27" s="6" t="s">
-        <v>11</v>
-      </c>
+      <c r="M27" s="15"/>
     </row>
     <row r="28" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F28" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>2</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="M28" s="16"/>
     </row>
     <row r="29" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M29" s="13"/>
+      <c r="F29" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="17"/>
     </row>
     <row r="30" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="8"/>
-      <c r="M30" s="13"/>
+      <c r="F30" s="7"/>
+      <c r="M30" s="17"/>
     </row>
     <row r="31" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F31" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="M31" s="13"/>
+        <v>13</v>
+      </c>
+      <c r="M31" s="17"/>
     </row>
     <row r="32" spans="4:13" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M32" s="13"/>
+      <c r="M32" s="17"/>
     </row>
     <row r="39" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="H39" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="40" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H40" s="14" t="s">
-        <v>3</v>
+      <c r="H40" s="11" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="41" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H41" s="15"/>
+      <c r="H41" s="12"/>
     </row>
     <row r="42" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H42" s="15"/>
+      <c r="H42" s="12"/>
     </row>
     <row r="43" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H43" s="15"/>
+      <c r="H43" s="12"/>
     </row>
     <row r="44" spans="8:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="H44" s="15"/>
+      <c r="H44" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="12">
     <mergeCell ref="D19:D23"/>
     <mergeCell ref="H19:H23"/>
-    <mergeCell ref="M28:M32"/>
     <mergeCell ref="H40:H44"/>
     <mergeCell ref="F13:F15"/>
     <mergeCell ref="F18:F19"/>

</xml_diff>